<commit_message>
irrigation sector update method done, planthealthGet method done, IrrigationTask stack size increased, statusNotify  stack size decreased
</commit_message>
<xml_diff>
--- a/IrrigationModule/StackHeapCalcs.xlsx
+++ b/IrrigationModule/StackHeapCalcs.xlsx
@@ -422,7 +422,7 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -486,8 +486,8 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <f>$B$2+128</f>
-        <v>256</v>
+        <f>$B$2+192</f>
+        <v>320</v>
       </c>
       <c r="H2">
         <f>$B$2</f>
@@ -527,7 +527,7 @@
       </c>
       <c r="G3">
         <f>G2*4</f>
-        <v>1024</v>
+        <v>1280</v>
       </c>
       <c r="H3">
         <f>H2*4</f>
@@ -567,7 +567,7 @@
       </c>
       <c r="G4">
         <f>G3/1024</f>
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="H4">
         <f>H3/1024</f>
@@ -587,7 +587,7 @@
       </c>
       <c r="N4">
         <f>B4+G4+H4+I4+J4+K4</f>
-        <v>3.5</v>
+        <v>3.75</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -626,7 +626,7 @@
       </c>
       <c r="E9">
         <f>D4+N4</f>
-        <v>7.5</v>
+        <v>7.75</v>
       </c>
       <c r="F9">
         <f>C4+E4</f>
@@ -634,7 +634,7 @@
       </c>
       <c r="G9" s="1">
         <f>E9+F9+4</f>
-        <v>35.5</v>
+        <v>35.75</v>
       </c>
       <c r="I9">
         <v>4</v>

</xml_diff>

<commit_message>
Wireless communication futher work, Message class implemented in place of structs for comm handling, style changes
</commit_message>
<xml_diff>
--- a/IrrigationModule/StackHeapCalcs.xlsx
+++ b/IrrigationModule/StackHeapCalcs.xlsx
@@ -422,7 +422,7 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -490,8 +490,8 @@
         <v>320</v>
       </c>
       <c r="H2">
-        <f>$B$2</f>
-        <v>128</v>
+        <f>$B$2+64</f>
+        <v>192</v>
       </c>
       <c r="I2">
         <f>$B$2</f>
@@ -531,7 +531,7 @@
       </c>
       <c r="H3">
         <f>H2*4</f>
-        <v>512</v>
+        <v>768</v>
       </c>
       <c r="I3">
         <f>I2*4</f>
@@ -571,7 +571,7 @@
       </c>
       <c r="H4">
         <f>H3/1024</f>
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="I4">
         <f>I3/1024</f>
@@ -587,7 +587,7 @@
       </c>
       <c r="N4">
         <f>B4+G4+H4+I4+J4+K4</f>
-        <v>3.75</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -626,7 +626,7 @@
       </c>
       <c r="E9">
         <f>D4+N4</f>
-        <v>7.75</v>
+        <v>8</v>
       </c>
       <c r="F9">
         <f>C4+E4</f>
@@ -634,7 +634,7 @@
       </c>
       <c r="G9" s="1">
         <f>E9+F9+4</f>
-        <v>35.75</v>
+        <v>36</v>
       </c>
       <c r="I9">
         <v>4</v>

</xml_diff>

<commit_message>
got rid of global using namespace in headers, plants queue bug corrected
</commit_message>
<xml_diff>
--- a/IrrigationModule/StackHeapCalcs.xlsx
+++ b/IrrigationModule/StackHeapCalcs.xlsx
@@ -422,7 +422,7 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -515,8 +515,8 @@
         <v>512</v>
       </c>
       <c r="C3">
-        <f>24*1024</f>
-        <v>24576</v>
+        <f>25*1024</f>
+        <v>25600</v>
       </c>
       <c r="D3" s="1">
         <f>4*D2</f>
@@ -556,7 +556,7 @@
       </c>
       <c r="C4">
         <f>C3/1024</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" s="1">
         <f>D3/1024</f>
@@ -622,7 +622,7 @@
       </c>
       <c r="D9">
         <f>E4+C4</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E9">
         <f>D4+N4</f>
@@ -630,11 +630,11 @@
       </c>
       <c r="F9">
         <f>C4+E4</f>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G9" s="1">
         <f>E9+F9+4</f>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I9">
         <v>4</v>

</xml_diff>

<commit_message>
major changes in memory layout, queues, sectors handling, hardfault errors tracking added to startup script
</commit_message>
<xml_diff>
--- a/IrrigationModule/StackHeapCalcs.xlsx
+++ b/IrrigationModule/StackHeapCalcs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>configIdletask stack</t>
   </si>
@@ -87,6 +87,21 @@
   </si>
   <si>
     <t>SRAM total avbl</t>
+  </si>
+  <si>
+    <t>wireless</t>
+  </si>
+  <si>
+    <t>irrigation</t>
+  </si>
+  <si>
+    <t>user button</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>adc</t>
   </si>
 </sst>
 </file>
@@ -422,7 +437,7 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -486,12 +501,12 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <f>$B$2+192</f>
-        <v>320</v>
+        <f>$B$2+256+256</f>
+        <v>640</v>
       </c>
       <c r="H2">
-        <f>$B$2+64</f>
-        <v>192</v>
+        <f>$B$2+256</f>
+        <v>384</v>
       </c>
       <c r="I2">
         <f>$B$2</f>
@@ -515,8 +530,8 @@
         <v>512</v>
       </c>
       <c r="C3">
-        <f>25*1024</f>
-        <v>25600</v>
+        <f>26*1024</f>
+        <v>26624</v>
       </c>
       <c r="D3" s="1">
         <f>4*D2</f>
@@ -527,11 +542,11 @@
       </c>
       <c r="G3">
         <f>G2*4</f>
-        <v>1280</v>
+        <v>2560</v>
       </c>
       <c r="H3">
         <f>H2*4</f>
-        <v>768</v>
+        <v>1536</v>
       </c>
       <c r="I3">
         <f>I2*4</f>
@@ -556,7 +571,7 @@
       </c>
       <c r="C4">
         <f>C3/1024</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D4" s="1">
         <f>D3/1024</f>
@@ -567,11 +582,11 @@
       </c>
       <c r="G4">
         <f>G3/1024</f>
-        <v>1.25</v>
+        <v>2.5</v>
       </c>
       <c r="H4">
         <f>H3/1024</f>
-        <v>0.75</v>
+        <v>1.5</v>
       </c>
       <c r="I4">
         <f>I3/1024</f>
@@ -587,7 +602,24 @@
       </c>
       <c r="N4">
         <f>B4+G4+H4+I4+J4+K4</f>
-        <v>4</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
@@ -622,19 +654,19 @@
       </c>
       <c r="D9">
         <f>E4+C4</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E9">
         <f>D4+N4</f>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F9">
         <f>C4+E4</f>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G9" s="1">
         <f>E9+F9+4</f>
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="I9">
         <v>4</v>

</xml_diff>

<commit_message>
stacks, heaps adjustments, ref voltages adjusted to new ldo 3.3v, handle confirmation moved to sector class
</commit_message>
<xml_diff>
--- a/IrrigationModule/StackHeapCalcs.xlsx
+++ b/IrrigationModule/StackHeapCalcs.xlsx
@@ -437,7 +437,7 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -501,12 +501,12 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <f>$B$2+256+256</f>
+        <f>$B$2+1408+384</f>
+        <v>1920</v>
+      </c>
+      <c r="H2">
+        <f>$B$2+512</f>
         <v>640</v>
-      </c>
-      <c r="H2">
-        <f>$B$2+256</f>
-        <v>384</v>
       </c>
       <c r="I2">
         <f>$B$2</f>
@@ -530,8 +530,8 @@
         <v>512</v>
       </c>
       <c r="C3">
-        <f>26*1024</f>
-        <v>26624</v>
+        <f>16*1024</f>
+        <v>16384</v>
       </c>
       <c r="D3" s="1">
         <f>4*D2</f>
@@ -542,11 +542,11 @@
       </c>
       <c r="G3">
         <f>G2*4</f>
-        <v>2560</v>
+        <v>7680</v>
       </c>
       <c r="H3">
         <f>H2*4</f>
-        <v>1536</v>
+        <v>2560</v>
       </c>
       <c r="I3">
         <f>I2*4</f>
@@ -571,7 +571,7 @@
       </c>
       <c r="C4">
         <f>C3/1024</f>
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1">
         <f>D3/1024</f>
@@ -582,11 +582,11 @@
       </c>
       <c r="G4">
         <f>G3/1024</f>
-        <v>2.5</v>
+        <v>7.5</v>
       </c>
       <c r="H4">
         <f>H3/1024</f>
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="I4">
         <f>I3/1024</f>
@@ -602,7 +602,7 @@
       </c>
       <c r="N4">
         <f>B4+G4+H4+I4+J4+K4</f>
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
@@ -654,19 +654,19 @@
       </c>
       <c r="D9">
         <f>E4+C4</f>
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="E9">
         <f>D4+N4</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F9">
         <f>C4+E4</f>
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="G9" s="1">
         <f>E9+F9+4</f>
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="I9">
         <v>4</v>

</xml_diff>